<commit_message>
Design - Security Mechanisms done
</commit_message>
<xml_diff>
--- a/Documentations/2 - Analysis/RiskAssessment.xlsx
+++ b/Documentations/2 - Analysis/RiskAssessment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4733ed64e92542de/Documents/School/3. semester/SEP3/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karrt\Desktop\All_Folders\Uni\Semester3\Semester Project Heterogeneous System (SEP3)\1 SEP3\SEP3XA20-ARS\Documentations\2 - Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:40000_{909C2352-02DB-4AFA-A5DD-3E30F39622CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BA78BF-B13B-47F4-ADAB-4A2D5D133A58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6165" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-27660" yWindow="0" windowWidth="27615" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Threat</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Exchanging public keys instead of using certificate authority</t>
   </si>
   <si>
-    <t>Use certificate authority</t>
-  </si>
-  <si>
     <t>Tampering</t>
   </si>
   <si>
@@ -159,13 +156,28 @@
   </si>
   <si>
     <t>Website. The website will be unavailable</t>
+  </si>
+  <si>
+    <t>Replay attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unencrypted </t>
+  </si>
+  <si>
+    <t>Data. The threat agent can intercept data while imposing as the genuine user</t>
+  </si>
+  <si>
+    <t>Use certificate authority and encryption</t>
+  </si>
+  <si>
+    <t>TLS (add sequence numbers and MACs to packages, and use nounces)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,18 +284,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -602,277 +617,298 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.109375" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" customWidth="1"/>
-    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="27.08984375" customWidth="1"/>
+    <col min="2" max="2" width="23.08984375" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="42" thickBot="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="210.6" customHeight="1">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" ht="210.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="13.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="6"/>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="13.2" customHeight="1" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="5"/>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="113.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="6"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="113.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="109.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="6"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" ht="76.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6"/>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="113.4" customHeight="1" thickBot="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="109.8" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="G9" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" ht="82.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G11" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="76.2" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="82.2" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="68.400000000000006" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="F13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A2:A6"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>